<commit_message>
Node Mailer working + Excell up and running
</commit_message>
<xml_diff>
--- a/backend/__tests__/users.xlsx
+++ b/backend/__tests__/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\WORK\Sopra\talentTracker\backend\__tests__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E54D8ADC-83A1-4812-AF93-51F8CE1F6D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A29BE3-CA79-4E75-B0EC-083FC8E6B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{18647FE5-393A-4605-9DA2-21C43EFC5316}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -44,16 +44,31 @@
     <t>password</t>
   </si>
   <si>
-    <t>akremgomri1@gmail.com</t>
-  </si>
-  <si>
     <t>Haroungomri@gmail.com</t>
   </si>
   <si>
     <t>azerty123</t>
   </si>
   <si>
-    <t>passwordConfirm</t>
+    <t>SafaAbid@gmail.com</t>
+  </si>
+  <si>
+    <t>azerty</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>gomriakrem1@gmail.com</t>
+  </si>
+  <si>
+    <t>achref.gomri@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -416,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B27A59-4062-472A-970F-DA648598442B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,35 +450,50 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{790D4A41-6697-4DE4-AA78-C25C354D7A11}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{0838C0C9-80B7-4DE7-9775-0B39CC1ABD41}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{83D10484-8638-478C-831B-36D5BCA725F1}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{3C8BED99-A2DC-4B1D-BF7A-F28AD33BDA6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>